<commit_message>
Removed dummy transcripts, updated liberal arts credits
</commit_message>
<xml_diff>
--- a/Students_test/blankPPF.xlsx
+++ b/Students_test/blankPPF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshpopp/Downloads/ppfproj/Students_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABBA443-4A05-6149-98C2-8C9A3CB44832}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA077EE-BDB0-7E45-A0B9-30F8FB38B635}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="460" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1100" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PPF 2007" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -568,6 +569,7 @@
     <font>
       <sz val="9"/>
       <name val="Monaco"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -750,68 +752,68 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1152,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -1174,123 +1176,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
       <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
       <c r="N3" s="2"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="68" t="s">
+      <c r="J5" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="68"/>
-      <c r="L5" s="78">
+      <c r="K5" s="59"/>
+      <c r="L5" s="60">
         <f ca="1">TODAY()</f>
-        <v>43505</v>
-      </c>
-      <c r="M5" s="78"/>
+        <v>43663</v>
+      </c>
+      <c r="M5" s="60"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="81" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="68" t="s">
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="68"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="68" t="s">
+      <c r="J7" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
       <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:14" ht="14" thickBot="1">
       <c r="A8" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
       <c r="J8" s="50" t="s">
         <v>31</v>
       </c>
@@ -1346,75 +1348,75 @@
       <c r="A11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="17"/>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="H12" s="67"/>
+      <c r="H12" s="64"/>
       <c r="I12" s="6"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="17"/>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="67" t="s">
+      <c r="G13" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="67"/>
+      <c r="H13" s="64"/>
       <c r="I13" s="7"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="17"/>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="67" t="s">
+      <c r="G14" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="67"/>
+      <c r="H14" s="64"/>
       <c r="I14" s="7"/>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="17"/>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="67" t="s">
+      <c r="G15" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="67"/>
+      <c r="H15" s="64"/>
       <c r="I15" s="7"/>
       <c r="K15" s="6"/>
       <c r="M15" s="6">
@@ -1424,13 +1426,13 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="17"/>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="17"/>
@@ -1439,43 +1441,43 @@
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="17"/>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="58"/>
+      <c r="H19" s="61"/>
       <c r="I19" s="6"/>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="17"/>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="58"/>
+      <c r="H20" s="61"/>
       <c r="I20" s="6"/>
       <c r="K20" s="7"/>
       <c r="M20" s="6">
@@ -1491,12 +1493,12 @@
       <c r="A22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
       <c r="F22" s="2"/>
       <c r="I22" s="8"/>
       <c r="J22" s="13"/>
@@ -1506,29 +1508,29 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="17"/>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="H23" s="58"/>
+      <c r="H23" s="61"/>
       <c r="I23" s="6"/>
       <c r="K23" s="6"/>
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="17"/>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
       <c r="G24" s="42" t="s">
         <v>61</v>
       </c>
@@ -1546,41 +1548,41 @@
       <c r="A26" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="17"/>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
       <c r="I27" s="6"/>
       <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="17"/>
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
       <c r="I28" s="7"/>
       <c r="K28" s="7"/>
     </row>
@@ -1593,8 +1595,8 @@
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="33"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
       <c r="I29" s="7"/>
       <c r="K29" s="7"/>
     </row>
@@ -1603,38 +1605,38 @@
       <c r="B30" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
       <c r="I30" s="7"/>
       <c r="J30" s="1"/>
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="17"/>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
       <c r="I31" s="8"/>
       <c r="J31" s="1"/>
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="17"/>
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
       <c r="I32" s="6"/>
       <c r="J32" s="1"/>
       <c r="K32" s="6"/>
@@ -1671,25 +1673,25 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="17"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
       <c r="I35" s="6"/>
       <c r="K35" s="6"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="17"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
       <c r="I36" s="7"/>
       <c r="K36" s="7"/>
       <c r="M36" s="6">
@@ -1714,20 +1716,20 @@
       <c r="A38" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="68" t="s">
+      <c r="B38" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="59"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="17"/>
@@ -1763,29 +1765,29 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="17"/>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="68"/>
       <c r="I41" s="8"/>
       <c r="K41" s="8"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="17"/>
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="68"/>
       <c r="I42" s="8"/>
       <c r="J42" s="13"/>
       <c r="K42" s="8"/>
@@ -1793,15 +1795,15 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="17"/>
-      <c r="B43" s="61" t="s">
+      <c r="B43" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="68"/>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
@@ -1809,15 +1811,15 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="17"/>
-      <c r="B44" s="61" t="s">
+      <c r="B44" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="68"/>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
@@ -1825,15 +1827,15 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="17"/>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
       <c r="I45" s="8"/>
       <c r="J45" s="13"/>
       <c r="K45" s="8"/>
@@ -1841,15 +1843,15 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="17"/>
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
+      <c r="C46" s="68"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="68"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="68"/>
       <c r="I46" s="8"/>
       <c r="J46" s="13"/>
       <c r="K46" s="8"/>
@@ -1866,73 +1868,73 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="17"/>
-      <c r="B48" s="58"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
       <c r="F48" s="34"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
       <c r="I48" s="8"/>
       <c r="J48" s="13"/>
       <c r="K48" s="8"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="17"/>
-      <c r="B49" s="62"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="62"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="64"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="84"/>
       <c r="H49" s="38"/>
       <c r="I49" s="36"/>
       <c r="K49" s="36"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="17"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="62"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="62"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="65"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="85"/>
       <c r="H50" s="38"/>
       <c r="I50" s="7"/>
       <c r="K50" s="7"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="17"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="62"/>
-      <c r="E51" s="62"/>
-      <c r="F51" s="65"/>
-      <c r="G51" s="65"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="85"/>
+      <c r="G51" s="85"/>
       <c r="H51" s="38"/>
       <c r="I51" s="7"/>
       <c r="K51" s="7"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="17"/>
-      <c r="B52" s="62"/>
-      <c r="C52" s="62"/>
-      <c r="D52" s="62"/>
-      <c r="E52" s="62"/>
-      <c r="F52" s="65"/>
-      <c r="G52" s="65"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="85"/>
       <c r="H52" s="38"/>
       <c r="I52" s="36"/>
       <c r="K52" s="36"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="17"/>
-      <c r="B53" s="62"/>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="62"/>
-      <c r="F53" s="65"/>
-      <c r="G53" s="65"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="85"/>
       <c r="H53" s="38"/>
       <c r="I53" s="36"/>
       <c r="J53" s="13"/>
@@ -1941,12 +1943,12 @@
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="17"/>
-      <c r="B54" s="62"/>
-      <c r="C54" s="62"/>
-      <c r="D54" s="62"/>
-      <c r="E54" s="62"/>
-      <c r="F54" s="65"/>
-      <c r="G54" s="65"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="85"/>
+      <c r="G54" s="85"/>
       <c r="H54" s="38"/>
       <c r="I54" s="7"/>
       <c r="K54" s="7"/>
@@ -1954,26 +1956,26 @@
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="17"/>
-      <c r="B55" s="61"/>
-      <c r="C55" s="61"/>
-      <c r="D55" s="61"/>
-      <c r="E55" s="61"/>
+      <c r="B55" s="68"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="68"/>
       <c r="F55" s="34"/>
-      <c r="G55" s="61"/>
-      <c r="H55" s="61"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="68"/>
       <c r="I55" s="8"/>
       <c r="K55" s="8"/>
       <c r="M55" s="8"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="17"/>
-      <c r="B56" s="69"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
+      <c r="B56" s="82"/>
+      <c r="C56" s="82"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="82"/>
+      <c r="F56" s="82"/>
+      <c r="G56" s="82"/>
+      <c r="H56" s="82"/>
       <c r="I56" s="8"/>
       <c r="J56" s="13"/>
       <c r="K56" s="8"/>
@@ -2027,13 +2029,13 @@
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="17"/>
-      <c r="B60" s="61"/>
-      <c r="C60" s="61"/>
-      <c r="D60" s="61"/>
-      <c r="E60" s="61"/>
+      <c r="B60" s="68"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="68"/>
+      <c r="E60" s="68"/>
       <c r="F60" s="19"/>
-      <c r="G60" s="61"/>
-      <c r="H60" s="61"/>
+      <c r="G60" s="68"/>
+      <c r="H60" s="68"/>
       <c r="I60" s="8"/>
       <c r="K60" s="8"/>
     </row>
@@ -2061,13 +2063,13 @@
       <c r="I62" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J62" s="71">
+      <c r="J62" s="78">
         <f>B5</f>
         <v>0</v>
       </c>
-      <c r="K62" s="71"/>
-      <c r="L62" s="71"/>
-      <c r="M62" s="71"/>
+      <c r="K62" s="78"/>
+      <c r="L62" s="78"/>
+      <c r="M62" s="78"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="17"/>
@@ -2088,27 +2090,27 @@
       <c r="A64" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="68" t="s">
+      <c r="B64" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="58"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="61"/>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="17"/>
-      <c r="B65" s="58" t="s">
+      <c r="B65" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
+      <c r="C65" s="61"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="61"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="60" t="s">
+      <c r="G65" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="H65" s="60"/>
+      <c r="H65" s="72"/>
       <c r="I65" s="6"/>
       <c r="K65" s="6"/>
       <c r="M65" s="6">
@@ -2123,8 +2125,8 @@
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="59"/>
+      <c r="G66" s="72"/>
+      <c r="H66" s="65"/>
       <c r="I66" s="53"/>
       <c r="K66" s="53"/>
     </row>
@@ -2158,93 +2160,93 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="17"/>
-      <c r="B69" s="66" t="s">
+      <c r="B69" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="C69" s="66"/>
-      <c r="D69" s="66"/>
-      <c r="E69" s="66"/>
-      <c r="F69" s="66"/>
-      <c r="G69" s="66"/>
-      <c r="H69" s="66"/>
+      <c r="C69" s="83"/>
+      <c r="D69" s="83"/>
+      <c r="E69" s="83"/>
+      <c r="F69" s="83"/>
+      <c r="G69" s="83"/>
+      <c r="H69" s="83"/>
       <c r="I69" s="13"/>
       <c r="K69" s="13"/>
     </row>
     <row r="70" spans="1:13" ht="15">
       <c r="A70" s="17"/>
-      <c r="B70" s="58" t="s">
+      <c r="B70" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
+      <c r="C70" s="61"/>
+      <c r="D70" s="61"/>
+      <c r="E70" s="61"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="58" t="s">
+      <c r="G70" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="H70" s="58"/>
+      <c r="H70" s="61"/>
       <c r="I70" s="6"/>
       <c r="K70" s="6"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="17"/>
-      <c r="B71" s="58" t="s">
+      <c r="B71" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
+      <c r="C71" s="61"/>
+      <c r="D71" s="61"/>
+      <c r="E71" s="61"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="58" t="s">
+      <c r="G71" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="H71" s="58"/>
+      <c r="H71" s="61"/>
       <c r="I71" s="7"/>
       <c r="K71" s="7"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="3"/>
-      <c r="B72" s="66" t="s">
+      <c r="B72" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="66"/>
-      <c r="D72" s="66"/>
-      <c r="E72" s="66"/>
-      <c r="F72" s="66"/>
-      <c r="G72" s="66"/>
-      <c r="H72" s="66"/>
+      <c r="C72" s="83"/>
+      <c r="D72" s="83"/>
+      <c r="E72" s="83"/>
+      <c r="F72" s="83"/>
+      <c r="G72" s="83"/>
+      <c r="H72" s="83"/>
       <c r="I72" s="13"/>
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="17"/>
-      <c r="B73" s="58" t="s">
+      <c r="B73" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="C73" s="58"/>
-      <c r="D73" s="58"/>
-      <c r="E73" s="58"/>
+      <c r="C73" s="61"/>
+      <c r="D73" s="61"/>
+      <c r="E73" s="61"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="58" t="s">
+      <c r="G73" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H73" s="58"/>
+      <c r="H73" s="61"/>
       <c r="I73" s="6"/>
       <c r="K73" s="6"/>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="17"/>
-      <c r="B74" s="58" t="s">
+      <c r="B74" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="58"/>
-      <c r="D74" s="58"/>
-      <c r="E74" s="58"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="61"/>
+      <c r="E74" s="61"/>
       <c r="F74" s="46"/>
-      <c r="G74" s="58" t="s">
+      <c r="G74" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="H74" s="58"/>
+      <c r="H74" s="61"/>
       <c r="I74" s="48"/>
       <c r="K74" s="48"/>
     </row>
@@ -2264,34 +2266,34 @@
     </row>
     <row r="76" spans="1:13" ht="13.5" customHeight="1">
       <c r="A76" s="17"/>
-      <c r="B76" s="61" t="s">
+      <c r="B76" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="61"/>
-      <c r="D76" s="61"/>
-      <c r="E76" s="61"/>
-      <c r="F76" s="61"/>
-      <c r="G76" s="61" t="s">
+      <c r="C76" s="68"/>
+      <c r="D76" s="68"/>
+      <c r="E76" s="68"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="H76" s="61"/>
+      <c r="H76" s="68"/>
       <c r="I76" s="7"/>
       <c r="J76" s="1"/>
       <c r="K76" s="7"/>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="17"/>
-      <c r="B77" s="58" t="s">
+      <c r="B77" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C77" s="58"/>
-      <c r="D77" s="58"/>
-      <c r="E77" s="58"/>
+      <c r="C77" s="61"/>
+      <c r="D77" s="61"/>
+      <c r="E77" s="61"/>
       <c r="F77" s="46"/>
-      <c r="G77" s="58" t="s">
+      <c r="G77" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="H77" s="58"/>
+      <c r="H77" s="61"/>
       <c r="I77" s="48"/>
       <c r="J77" s="1"/>
       <c r="K77" s="48"/>
@@ -2304,59 +2306,59 @@
       <c r="D78" s="47"/>
       <c r="E78" s="47"/>
       <c r="F78" s="47"/>
-      <c r="G78" s="61" t="s">
+      <c r="G78" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="H78" s="61"/>
+      <c r="H78" s="68"/>
       <c r="I78" s="48"/>
       <c r="J78" s="1"/>
       <c r="K78" s="48"/>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="17"/>
-      <c r="B79" s="58" t="s">
+      <c r="B79" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="C79" s="58"/>
-      <c r="D79" s="58"/>
-      <c r="E79" s="58"/>
+      <c r="C79" s="61"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="61"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="58" t="s">
+      <c r="G79" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="H79" s="58"/>
+      <c r="H79" s="61"/>
       <c r="I79" s="6"/>
       <c r="K79" s="6"/>
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="17"/>
-      <c r="B80" s="58" t="s">
+      <c r="B80" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="C80" s="58"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="58"/>
+      <c r="C80" s="61"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="61"/>
       <c r="F80" s="2"/>
-      <c r="G80" s="58" t="s">
+      <c r="G80" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="H80" s="58"/>
+      <c r="H80" s="61"/>
       <c r="I80" s="8"/>
       <c r="K80" s="8"/>
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="17"/>
-      <c r="B81" s="58" t="s">
+      <c r="B81" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="C81" s="58"/>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="61"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="58" t="s">
+      <c r="G81" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="H81" s="58"/>
+      <c r="H81" s="61"/>
       <c r="I81" s="7"/>
       <c r="K81" s="7"/>
     </row>
@@ -2373,70 +2375,70 @@
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="17"/>
-      <c r="B83" s="58" t="s">
+      <c r="B83" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="C83" s="58"/>
-      <c r="D83" s="58"/>
-      <c r="E83" s="58"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="58"/>
-      <c r="H83" s="58"/>
-      <c r="I83" s="59"/>
-      <c r="J83" s="59"/>
-      <c r="K83" s="59"/>
+      <c r="C83" s="61"/>
+      <c r="D83" s="61"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="61"/>
+      <c r="H83" s="61"/>
+      <c r="I83" s="65"/>
+      <c r="J83" s="65"/>
+      <c r="K83" s="65"/>
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="17"/>
-      <c r="B84" s="58" t="s">
+      <c r="B84" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="C84" s="58"/>
-      <c r="D84" s="58"/>
-      <c r="E84" s="58"/>
+      <c r="C84" s="61"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="61"/>
       <c r="F84" s="2"/>
-      <c r="G84" s="58"/>
-      <c r="H84" s="58"/>
+      <c r="G84" s="61"/>
+      <c r="H84" s="61"/>
       <c r="I84" s="6"/>
       <c r="J84" s="1"/>
       <c r="K84" s="6"/>
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="17"/>
-      <c r="B85" s="58" t="s">
+      <c r="B85" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="C85" s="58"/>
-      <c r="D85" s="58"/>
-      <c r="E85" s="58"/>
+      <c r="C85" s="61"/>
+      <c r="D85" s="61"/>
+      <c r="E85" s="61"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="58"/>
-      <c r="H85" s="58"/>
+      <c r="G85" s="61"/>
+      <c r="H85" s="61"/>
       <c r="I85" s="6"/>
       <c r="K85" s="6"/>
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="17"/>
-      <c r="B86" s="58" t="s">
+      <c r="B86" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="C86" s="58"/>
-      <c r="D86" s="58"/>
-      <c r="E86" s="58"/>
+      <c r="C86" s="61"/>
+      <c r="D86" s="61"/>
+      <c r="E86" s="61"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="58"/>
-      <c r="H86" s="58"/>
+      <c r="G86" s="61"/>
+      <c r="H86" s="61"/>
       <c r="I86" s="6"/>
       <c r="K86" s="6"/>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="17"/>
-      <c r="B87" s="58" t="s">
+      <c r="B87" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="C87" s="58"/>
-      <c r="D87" s="58"/>
-      <c r="E87" s="58"/>
+      <c r="C87" s="61"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="61"/>
       <c r="F87" s="46"/>
       <c r="G87" s="46"/>
       <c r="H87" s="46"/>
@@ -2445,12 +2447,12 @@
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="17"/>
-      <c r="B88" s="58" t="s">
+      <c r="B88" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="58"/>
-      <c r="D88" s="58"/>
-      <c r="E88" s="58"/>
+      <c r="C88" s="61"/>
+      <c r="D88" s="61"/>
+      <c r="E88" s="61"/>
       <c r="F88" s="46"/>
       <c r="G88" s="46"/>
       <c r="H88" s="46"/>
@@ -2459,25 +2461,25 @@
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="17"/>
-      <c r="B89" s="58"/>
-      <c r="C89" s="58"/>
-      <c r="D89" s="58"/>
-      <c r="E89" s="58"/>
-      <c r="F89" s="59"/>
-      <c r="G89" s="58"/>
-      <c r="H89" s="58"/>
+      <c r="B89" s="61"/>
+      <c r="C89" s="61"/>
+      <c r="D89" s="61"/>
+      <c r="E89" s="61"/>
+      <c r="F89" s="65"/>
+      <c r="G89" s="61"/>
+      <c r="H89" s="61"/>
       <c r="I89" s="7"/>
       <c r="K89" s="7"/>
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="17"/>
-      <c r="B90" s="58"/>
-      <c r="C90" s="58"/>
-      <c r="D90" s="58"/>
-      <c r="E90" s="58"/>
-      <c r="F90" s="59"/>
-      <c r="G90" s="58"/>
-      <c r="H90" s="58"/>
+      <c r="B90" s="61"/>
+      <c r="C90" s="61"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="61"/>
+      <c r="F90" s="65"/>
+      <c r="G90" s="61"/>
+      <c r="H90" s="61"/>
       <c r="I90" s="7"/>
       <c r="K90" s="7"/>
       <c r="M90" s="6">
@@ -2492,47 +2494,47 @@
       <c r="A92" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="68" t="s">
+      <c r="B92" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C92" s="58"/>
-      <c r="D92" s="58"/>
-      <c r="E92" s="58"/>
+      <c r="C92" s="61"/>
+      <c r="D92" s="61"/>
+      <c r="E92" s="61"/>
       <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="17"/>
-      <c r="B93" s="58"/>
-      <c r="C93" s="58"/>
-      <c r="D93" s="58"/>
-      <c r="E93" s="58"/>
-      <c r="F93" s="59"/>
-      <c r="G93" s="72"/>
-      <c r="H93" s="72"/>
+      <c r="B93" s="61"/>
+      <c r="C93" s="61"/>
+      <c r="D93" s="61"/>
+      <c r="E93" s="61"/>
+      <c r="F93" s="65"/>
+      <c r="G93" s="80"/>
+      <c r="H93" s="80"/>
       <c r="I93" s="32"/>
       <c r="K93" s="6"/>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="17"/>
-      <c r="B94" s="58"/>
-      <c r="C94" s="58"/>
-      <c r="D94" s="58"/>
-      <c r="E94" s="58"/>
-      <c r="F94" s="59"/>
-      <c r="G94" s="58"/>
-      <c r="H94" s="58"/>
+      <c r="B94" s="61"/>
+      <c r="C94" s="61"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
+      <c r="F94" s="65"/>
+      <c r="G94" s="61"/>
+      <c r="H94" s="61"/>
       <c r="I94" s="6"/>
       <c r="K94" s="6"/>
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="17"/>
-      <c r="B95" s="58"/>
-      <c r="C95" s="58"/>
-      <c r="D95" s="58"/>
-      <c r="E95" s="58"/>
-      <c r="F95" s="59"/>
-      <c r="G95" s="58"/>
-      <c r="H95" s="58"/>
+      <c r="B95" s="61"/>
+      <c r="C95" s="61"/>
+      <c r="D95" s="61"/>
+      <c r="E95" s="61"/>
+      <c r="F95" s="65"/>
+      <c r="G95" s="61"/>
+      <c r="H95" s="61"/>
       <c r="I95" s="7"/>
       <c r="K95" s="7"/>
       <c r="M95" s="6">
@@ -2555,16 +2557,16 @@
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="17"/>
-      <c r="B97" s="58"/>
-      <c r="C97" s="58"/>
-      <c r="D97" s="58"/>
-      <c r="E97" s="58"/>
-      <c r="F97" s="58"/>
-      <c r="G97" s="58"/>
-      <c r="H97" s="58"/>
-      <c r="I97" s="58"/>
-      <c r="J97" s="58"/>
-      <c r="K97" s="58"/>
+      <c r="B97" s="61"/>
+      <c r="C97" s="61"/>
+      <c r="D97" s="61"/>
+      <c r="E97" s="61"/>
+      <c r="F97" s="61"/>
+      <c r="G97" s="61"/>
+      <c r="H97" s="61"/>
+      <c r="I97" s="61"/>
+      <c r="J97" s="61"/>
+      <c r="K97" s="61"/>
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="17"/>
@@ -2583,49 +2585,49 @@
       <c r="A99" s="17"/>
       <c r="J99" s="23"/>
       <c r="K99" s="25"/>
-      <c r="L99" s="70" t="s">
+      <c r="L99" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="M99" s="70"/>
+      <c r="M99" s="77"/>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="17"/>
       <c r="B100" s="6"/>
-      <c r="C100" s="58" t="s">
+      <c r="C100" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="D100" s="58"/>
-      <c r="E100" s="59"/>
-      <c r="F100" s="59"/>
-      <c r="G100" s="59"/>
-      <c r="H100" s="63"/>
-      <c r="I100" s="63"/>
+      <c r="D100" s="61"/>
+      <c r="E100" s="65"/>
+      <c r="F100" s="65"/>
+      <c r="G100" s="65"/>
+      <c r="H100" s="79"/>
+      <c r="I100" s="79"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="17"/>
       <c r="B101" s="7"/>
-      <c r="C101" s="58" t="s">
+      <c r="C101" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="D101" s="58"/>
-      <c r="E101" s="58"/>
-      <c r="F101" s="58"/>
-      <c r="G101" s="58"/>
-      <c r="H101" s="63"/>
-      <c r="I101" s="63"/>
+      <c r="D101" s="61"/>
+      <c r="E101" s="61"/>
+      <c r="F101" s="61"/>
+      <c r="G101" s="61"/>
+      <c r="H101" s="79"/>
+      <c r="I101" s="79"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="17"/>
       <c r="B102" s="7"/>
-      <c r="C102" s="58" t="s">
+      <c r="C102" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="D102" s="59"/>
-      <c r="E102" s="59"/>
-      <c r="F102" s="59"/>
-      <c r="G102" s="59"/>
-      <c r="H102" s="63"/>
-      <c r="I102" s="63"/>
+      <c r="D102" s="65"/>
+      <c r="E102" s="65"/>
+      <c r="F102" s="65"/>
+      <c r="G102" s="65"/>
+      <c r="H102" s="79"/>
+      <c r="I102" s="79"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="17"/>
@@ -2633,12 +2635,12 @@
     <row r="104" spans="1:13">
       <c r="A104" s="17"/>
       <c r="B104" s="6"/>
-      <c r="C104" s="67" t="s">
+      <c r="C104" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="D104" s="67"/>
-      <c r="E104" s="67"/>
-      <c r="F104" s="67"/>
+      <c r="D104" s="64"/>
+      <c r="E104" s="64"/>
+      <c r="F104" s="64"/>
       <c r="G104" s="52"/>
       <c r="H104" s="3" t="s">
         <v>109</v>
@@ -2723,6 +2725,113 @@
     </row>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="B83:K83"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="C104:F104"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="B97:K97"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G29:H29"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2747,113 +2856,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="B97:K97"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="B84:E84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G95:H95"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="C104:F104"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="B83:K83"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="B72:H72"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>